<commit_message>
- added : footer last update info live updated
</commit_message>
<xml_diff>
--- a/public/data/db_source/info.xlsx
+++ b/public/data/db_source/info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannuaire/datannuaire_dev/db/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E743952-3289-8942-951A-B49C13472650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C334F87-E7E9-7543-829F-33FDAF65EA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,9 +398,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -415,7 +420,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1710083438</v>
+        <v>1728846186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>